<commit_message>
Update on 30th April after
</commit_message>
<xml_diff>
--- a/DB and Documents/MSCForm3.xlsx
+++ b/DB and Documents/MSCForm3.xlsx
@@ -234,9 +234,6 @@
     <t>q51z3</t>
   </si>
   <si>
-    <t>Maternal Sample Collection Form – Section 2: Vital Signs Data Collection</t>
-  </si>
-  <si>
     <t>5.Mother Full Name</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>10. Estimate of Blood Volume Collected in Tube. |__|.|__|ml</t>
+  </si>
+  <si>
+    <t>Maternal Sample Collection Form – Section 3: Blood Sample Collection</t>
   </si>
 </sst>
 </file>
@@ -1865,7 +1865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V2" sqref="V2:V41"/>
     </sheetView>
   </sheetViews>
@@ -1996,7 +1996,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="13"/>
       <c r="F3" s="18" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>62</v>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="V3" s="16" t="str">
         <f t="shared" ref="V3:V41" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'msg1','frmmessage', '','','Maternal Sample Collection Form – Section 2: Vital Signs Data Collection','','q2_3','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'msg1','frmmessage', '','','Maternal Sample Collection Form – Section 3: Blood Sample Collection','','q2_3','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="31.5">
@@ -2103,7 +2103,7 @@
         <v>36</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>47</v>
@@ -2137,7 +2137,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>48</v>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>49</v>
@@ -2205,7 +2205,7 @@
         <v>36</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>50</v>
@@ -2239,7 +2239,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>51</v>
@@ -2273,7 +2273,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>52</v>
@@ -2307,7 +2307,7 @@
         <v>36</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>53</v>
@@ -2332,7 +2332,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>30</v>
@@ -2342,7 +2342,7 @@
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>53</v>
@@ -2375,7 +2375,7 @@
         <v>36</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>54</v>
@@ -2409,7 +2409,7 @@
         <v>36</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>55</v>
@@ -2443,7 +2443,7 @@
         <v>36</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>56</v>
@@ -2477,7 +2477,7 @@
         <v>36</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" s="16" t="s">
         <v>57</v>
@@ -2505,13 +2505,13 @@
         <v>57</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>36</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>58</v>
@@ -2545,10 +2545,10 @@
         <v>36</v>
       </c>
       <c r="F19" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="16" t="s">
         <v>92</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>93</v>
       </c>
       <c r="R19" s="16" t="s">
         <v>33</v>
@@ -2570,7 +2570,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>29</v>
@@ -2579,10 +2579,10 @@
         <v>36</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R20" s="16" t="s">
         <v>33</v>
@@ -2604,7 +2604,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>29</v>
@@ -2613,10 +2613,10 @@
         <v>36</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R21" s="16" t="s">
         <v>33</v>
@@ -2638,7 +2638,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>31</v>
@@ -2647,10 +2647,10 @@
         <v>36</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R22" s="16" t="s">
         <v>33</v>
@@ -2672,7 +2672,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>29</v>
@@ -2681,11 +2681,11 @@
         <v>36</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R23" s="16" t="s">
         <v>33</v>
@@ -2707,7 +2707,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>29</v>
@@ -2716,11 +2716,11 @@
         <v>36</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R24" s="16" t="s">
         <v>33</v>
@@ -2742,7 +2742,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>31</v>
@@ -2751,11 +2751,11 @@
         <v>36</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R25" s="16" t="s">
         <v>33</v>
@@ -2777,7 +2777,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>29</v>
@@ -2786,10 +2786,10 @@
         <v>36</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R26" s="16" t="s">
         <v>33</v>
@@ -2811,7 +2811,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>29</v>
@@ -2820,10 +2820,10 @@
         <v>36</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R27" s="16" t="s">
         <v>33</v>
@@ -2845,7 +2845,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>31</v>
@@ -2854,10 +2854,10 @@
         <v>36</v>
       </c>
       <c r="F28" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="16" t="s">
         <v>109</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="R28" s="16" t="s">
         <v>33</v>
@@ -2879,7 +2879,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>29</v>
@@ -2888,10 +2888,10 @@
         <v>36</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R29" s="16" t="s">
         <v>33</v>
@@ -2913,7 +2913,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>29</v>
@@ -2922,10 +2922,10 @@
         <v>36</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R30" s="16" t="s">
         <v>33</v>
@@ -2947,7 +2947,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>31</v>
@@ -2956,10 +2956,10 @@
         <v>36</v>
       </c>
       <c r="F31" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="R31" s="16" t="s">
         <v>33</v>
@@ -2981,7 +2981,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>29</v>
@@ -2990,10 +2990,10 @@
         <v>36</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R32" s="16" t="s">
         <v>33</v>
@@ -3015,7 +3015,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>29</v>
@@ -3024,10 +3024,10 @@
         <v>36</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R33" s="16" t="s">
         <v>33</v>
@@ -3049,7 +3049,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>31</v>
@@ -3058,10 +3058,10 @@
         <v>36</v>
       </c>
       <c r="F34" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H34" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="R34" s="16" t="s">
         <v>33</v>
@@ -3083,7 +3083,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>29</v>
@@ -3092,10 +3092,10 @@
         <v>36</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R35" s="16" t="s">
         <v>33</v>
@@ -3117,7 +3117,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>29</v>
@@ -3126,10 +3126,10 @@
         <v>36</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R36" s="16" t="s">
         <v>33</v>
@@ -3151,7 +3151,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>31</v>
@@ -3160,10 +3160,10 @@
         <v>36</v>
       </c>
       <c r="F37" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H37" s="16" t="s">
         <v>127</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>128</v>
       </c>
       <c r="R37" s="16" t="s">
         <v>33</v>
@@ -3185,7 +3185,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>29</v>
@@ -3195,10 +3195,10 @@
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R38" s="16" t="s">
         <v>33</v>
@@ -3220,7 +3220,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>29</v>
@@ -3229,10 +3229,10 @@
         <v>36</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R39" s="16" t="s">
         <v>33</v>
@@ -3254,7 +3254,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>31</v>
@@ -3263,7 +3263,7 @@
         <v>36</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H40" s="16" t="s">
         <v>59</v>
@@ -3297,7 +3297,7 @@
         <v>36</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H41" s="16" t="s">
         <v>40</v>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="C2"/>
       <c r="D2" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="C3"/>
       <c r="D3" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="C4"/>
       <c r="D4" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="C5"/>
       <c r="D5" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="C6"/>
       <c r="D6" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -3718,7 +3718,7 @@
       </c>
       <c r="C7"/>
       <c r="D7" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="C8"/>
       <c r="D8" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="C9"/>
       <c r="D9" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="C10"/>
       <c r="D10" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="C11"/>
       <c r="D11" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -3816,13 +3816,13 @@
       </c>
       <c r="C12"/>
       <c r="D12" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3872,11 +3872,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15"/>
       <c r="D15" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3891,11 +3891,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16"/>
       <c r="D16" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -3910,11 +3910,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17"/>
       <c r="D17" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -3929,11 +3929,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18"/>
       <c r="D18" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="16">
         <v>1</v>
@@ -3948,11 +3948,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19"/>
       <c r="D19" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E19" s="16">
         <v>2</v>
@@ -3967,11 +3967,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20"/>
       <c r="D20" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E20" s="16">
         <v>3</v>
@@ -3986,11 +3986,11 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21"/>
       <c r="D21" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E21" s="16">
         <v>1</v>
@@ -4005,11 +4005,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22"/>
       <c r="D22" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E22" s="16">
         <v>2</v>
@@ -4024,11 +4024,11 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23"/>
       <c r="D23" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E23" s="16">
         <v>3</v>
@@ -4043,11 +4043,11 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24"/>
       <c r="D24" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="16">
         <v>1</v>
@@ -4062,11 +4062,11 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25"/>
       <c r="D25" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E25" s="16">
         <v>2</v>
@@ -4081,11 +4081,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26"/>
       <c r="D26" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26" s="16">
         <v>3</v>
@@ -4100,11 +4100,11 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27"/>
       <c r="D27" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" s="16">
         <v>1</v>
@@ -4119,11 +4119,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C28"/>
       <c r="D28" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" s="16">
         <v>2</v>
@@ -4138,11 +4138,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29"/>
       <c r="D29" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E29" s="16">
         <v>3</v>
@@ -4157,11 +4157,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30"/>
       <c r="D30" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" s="16">
         <v>1</v>
@@ -4176,11 +4176,11 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31"/>
       <c r="D31" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E31" s="16">
         <v>2</v>
@@ -4195,11 +4195,11 @@
         <v>31</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C32"/>
       <c r="D32" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E32" s="16">
         <v>3</v>
@@ -4214,11 +4214,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33"/>
       <c r="D33" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E33" s="16">
         <v>1</v>
@@ -4233,11 +4233,11 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34"/>
       <c r="D34" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" s="16">
         <v>2</v>
@@ -4252,11 +4252,11 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C35"/>
       <c r="D35" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" s="16">
         <v>3</v>

</xml_diff>